<commit_message>
Modificamos readme y certificados.py
Hice un par de modificaciones para que, a mi entender, sea más fácil utilizar el generador de certificados.
</commit_message>
<xml_diff>
--- a/certificados.xlsx
+++ b/certificados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ariel\Documents\GitHub\certificate-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fran\IEEE\certificate-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B88441E-DC88-4C24-9814-40A5C9F62954}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21AB97C-4DE5-4004-B1A4-F45C2E4FCF32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Ariel Nowik</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Nombre Certificado</t>
+  </si>
+  <si>
+    <t>Matias Sebastian Lopez Martinez</t>
   </si>
 </sst>
 </file>
@@ -364,13 +367,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
@@ -408,6 +411,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>